<commit_message>
Added tests for osapuolenrooli
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="127">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -122,12 +122,27 @@
     <t xml:space="preserve">041</t>
   </si>
   <si>
+    <t xml:space="preserve">100456789B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09800100010001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talovuori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">011</t>
+  </si>
+  <si>
     <t xml:space="preserve">123456789A</t>
   </si>
   <si>
-    <t xml:space="preserve">01</t>
-  </si>
-  <si>
     <t xml:space="preserve">039</t>
   </si>
   <si>
@@ -161,13 +176,16 @@
     <t xml:space="preserve">Okänt</t>
   </si>
   <si>
+    <t xml:space="preserve">Kuvakalliontie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAHTI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAHTIS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Harjukatu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAHTI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAHTIS</t>
   </si>
   <si>
     <t xml:space="preserve">Henkilötunnus</t>
@@ -264,6 +282,18 @@
     <t xml:space="preserve">Kerava</t>
   </si>
   <si>
+    <t xml:space="preserve">170467-8956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forsström Eino Einari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuvakalliontie 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">123456-0</t>
   </si>
   <si>
@@ -301,6 +331,15 @@
   </si>
   <si>
     <t xml:space="preserve">Tilapäisten asukk lukumäärä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forsström</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eino Einari</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -471,7 +510,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -480,6 +519,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -500,56 +543,56 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -629,224 +672,295 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="22.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>28341100010174</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>28341100010174</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="G2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="2" t="n">
         <v>19700101</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="0" t="n">
+      <c r="L2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="n">
         <v>280</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="2" t="n">
         <v>19910101</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="X2" s="0" t="n">
+      <c r="V2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" s="2" t="n">
         <v>6767693</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Y2" s="2" t="n">
         <v>400125</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="Z2" s="2" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>20000101</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>20010101</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2" t="n">
+        <v>6769404</v>
+      </c>
+      <c r="Y3" s="2" t="n">
+        <v>432590</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C4" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="n">
+      <c r="D4" s="8" t="n">
         <v>39800100010001</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F4" s="8" t="n">
         <v>39800100010001</v>
       </c>
-      <c r="G3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="n">
+      <c r="G4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="K3" s="8" t="n">
+      <c r="K4" s="9" t="n">
         <v>19800101</v>
       </c>
-      <c r="L3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N3" s="8" t="n">
+      <c r="L4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="9" t="n">
         <v>1000</v>
       </c>
-      <c r="O3" s="8" t="n">
+      <c r="O4" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="P3" s="8" t="n">
+      <c r="P4" s="9" t="n">
         <v>1500</v>
       </c>
-      <c r="Q3" s="8" t="n">
+      <c r="Q4" s="9" t="n">
         <v>4500</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T3" s="8" t="n">
+      <c r="S4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="9" t="n">
         <v>19800101</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="W3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="X3" s="8" t="n">
+      <c r="U4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="9" t="n">
         <v>6761402</v>
       </c>
-      <c r="Y3" s="8" t="n">
+      <c r="Y4" s="9" t="n">
         <v>427353</v>
       </c>
     </row>
@@ -866,100 +980,128 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="H3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="B4" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="9" t="n">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>398</v>
-      </c>
-      <c r="C3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="8" t="n">
-        <v>44</v>
-      </c>
-      <c r="G3" s="1" t="n">
+      <c r="G4" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>47</v>
+      <c r="H4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -978,174 +1120,219 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="D1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="E1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="I1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="K1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="M1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="N1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="O1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="P1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Q1" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="R1" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="S1" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="F2" s="8" t="n">
+      <c r="C2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="F2" s="9" t="n">
         <v>19950101</v>
       </c>
-      <c r="G2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="0" t="n">
+      <c r="G2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>444</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" s="0" t="n">
+      <c r="K2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="F3" s="9" t="n">
+        <v>20220101</v>
+      </c>
+      <c r="G3" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="I3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>20220101</v>
+      </c>
+      <c r="Q3" s="9"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="8" t="n">
+      <c r="D4" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="9" t="n">
         <v>20100101</v>
       </c>
-      <c r="G3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="16" t="s">
+      <c r="G4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="R3" s="1" t="n">
+      <c r="I4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="S3" s="8" t="s">
-        <v>82</v>
+      <c r="S4" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1164,238 +1351,281 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="18" t="s">
+      <c r="H2" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>398</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>15100</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="8" t="n">
-        <v>20200101</v>
-      </c>
-      <c r="N2" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="O2" s="8" t="n">
+      <c r="K2" s="20" t="n">
+        <v>15230</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>20220101</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>32</v>
+      <c r="A3" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>92</v>
+      <c r="C3" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>102</v>
+        <v>106</v>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="8" t="n">
-        <v>20210101</v>
-      </c>
-      <c r="N3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" s="8" t="n">
+      <c r="L3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="9" t="n">
+        <v>20200101</v>
+      </c>
+      <c r="N3" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="O3" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>32</v>
+      <c r="A4" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>103</v>
+      <c r="C4" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>108</v>
+        <v>111</v>
+      </c>
+      <c r="F4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="8" t="n">
-        <v>20220101</v>
-      </c>
-      <c r="N4" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="O4" s="8" t="n">
+      <c r="L4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="9" t="n">
+        <v>20210101</v>
+      </c>
+      <c r="N4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>32</v>
+      <c r="A5" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>103</v>
+      <c r="C5" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="F5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" s="8" t="n">
+      <c r="L5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="9" t="n">
+        <v>20220101</v>
+      </c>
+      <c r="N5" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O5" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>15100</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="9" t="n">
         <v>20220601</v>
       </c>
-      <c r="N5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8" t="n">
+      <c r="N6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed tests, Huo-neisto-kirjain and Jako-kirjain must include space instead of empty cells, import_dvv_kohteet needs loppupvm
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="128">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tilapäisten asukk lukumäärä</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">000</t>
@@ -416,7 +419,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -443,11 +446,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -510,7 +508,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -555,10 +553,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -585,14 +579,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -859,19 +845,19 @@
       <c r="L3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="N3" s="2" t="n">
         <v>300</v>
       </c>
-      <c r="O3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="P3" s="0" t="n">
+      <c r="O3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2" t="n">
         <v>300</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="2" t="n">
         <v>600</v>
       </c>
       <c r="S3" s="8" t="s">
@@ -989,7 +975,7 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -1052,7 +1038,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1129,7 +1115,7 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.53"/>
   </cols>
@@ -1144,7 +1130,7 @@
       <c r="C1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>55</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -1159,13 +1145,13 @@
       <c r="H1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>60</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>62</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -1189,22 +1175,22 @@
       <c r="R1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>73</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1260,7 +1246,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1354,14 +1340,14 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="23.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -1384,13 +1370,13 @@
       <c r="F1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>98</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -1405,51 +1391,57 @@
       <c r="M1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>102</v>
+      </c>
       <c r="D2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="19" t="s">
+      <c r="F2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>85</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="I2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K2" s="20" t="n">
+      <c r="K2" s="8" t="n">
         <v>15230</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="2" t="n">
         <v>20220101</v>
       </c>
-      <c r="N2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" s="0" t="n">
+      <c r="N2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1461,25 +1453,28 @@
         <v>398</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="F3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
@@ -1505,25 +1500,28 @@
         <v>398</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
@@ -1549,25 +1547,28 @@
         <v>398</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="F5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
@@ -1593,25 +1594,28 @@
         <v>398</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="F6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>

</xml_diff>

<commit_message>
Merged test Excel file manually and fixed tests
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="137">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -146,6 +146,12 @@
     <t xml:space="preserve">039</t>
   </si>
   <si>
+    <t xml:space="preserve">200000000A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">398</t>
+  </si>
+  <si>
     <t xml:space="preserve">Osoite-numero</t>
   </si>
   <si>
@@ -186,6 +192,9 @@
   </si>
   <si>
     <t xml:space="preserve">Harjukatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halmekatu</t>
   </si>
   <si>
     <t xml:space="preserve">Henkilötunnus</t>
@@ -306,6 +315,12 @@
     <t xml:space="preserve">Lahti</t>
   </si>
   <si>
+    <t xml:space="preserve">010440-865A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granström Otto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huo-neisto-kirjain</t>
   </si>
   <si>
@@ -409,6 +424,18 @@
   </si>
   <si>
     <t xml:space="preserve">Harjukatu 44 B 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">010655-3210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kemp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halmekatu 9</t>
   </si>
 </sst>
 </file>
@@ -658,10 +685,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -948,6 +975,68 @@
       </c>
       <c r="Y4" s="9" t="n">
         <v>427353</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>39800200010001</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>39800200010001</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>19750101</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <v>250</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>19780101</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2" t="n">
+        <v>6765134</v>
+      </c>
+      <c r="Y5" s="2" t="n">
+        <v>428759</v>
       </c>
     </row>
   </sheetData>
@@ -966,10 +1055,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -987,25 +1076,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,10 +1108,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -1031,10 +1120,10 @@
         <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
@@ -1058,10 +1147,10 @@
         <v>35</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>44</v>
@@ -1084,10 +1173,36 @@
         <v>15100</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1106,16 +1221,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.53"/>
   </cols>
@@ -1128,70 +1242,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,7 +1316,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D2" s="9"/>
       <c r="F2" s="9" t="n">
@@ -1212,37 +1326,37 @@
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,7 +1367,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D3" s="9"/>
       <c r="F3" s="9" t="n">
@@ -1263,25 +1377,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
@@ -1297,7 +1411,7 @@
         <v>398</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>20100101</v>
@@ -1309,16 +1423,45 @@
         <v>30</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>20010601</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>398</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1337,16 +1480,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="23.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.53"/>
   </cols>
@@ -1359,43 +1502,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,35 +1548,35 @@
       <c r="B2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>102</v>
+      <c r="C2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K2" s="8" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -1453,34 +1596,34 @@
         <v>398</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>102</v>
-      </c>
       <c r="F3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="M3" s="9" t="n">
         <v>20200101</v>
@@ -1500,34 +1643,34 @@
         <v>398</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>102</v>
+        <v>117</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="M4" s="9" t="n">
         <v>20210101</v>
@@ -1547,34 +1690,34 @@
         <v>398</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>123</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="M5" s="9" t="n">
         <v>20220101</v>
@@ -1594,34 +1737,34 @@
         <v>398</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>102</v>
+        <v>128</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="M6" s="9" t="n">
         <v>20220601</v>
@@ -1630,6 +1773,53 @@
         <v>1</v>
       </c>
       <c r="O6" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>20150401</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" s="2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added paritalokohde to tests
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="150">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -146,6 +146,24 @@
     <t xml:space="preserve">039</t>
   </si>
   <si>
+    <t xml:space="preserve">134567890B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VÄLIPURO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
     <t xml:space="preserve">200000000A</t>
   </si>
   <si>
@@ -192,6 +210,15 @@
   </si>
   <si>
     <t xml:space="preserve">Harjukatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirkkoäyrääntie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTJÄRVI</t>
   </si>
   <si>
     <t xml:space="preserve">Halmekatu</t>
@@ -315,6 +342,15 @@
     <t xml:space="preserve">Lahti</t>
   </si>
   <si>
+    <t xml:space="preserve">151045-9873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lindroth John Johan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirkkoäyrääntie 1d</t>
+  </si>
+  <si>
     <t xml:space="preserve">010440-865A</t>
   </si>
   <si>
@@ -360,9 +396,6 @@
     <t xml:space="preserve">Eino Einari</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
     <t xml:space="preserve">001</t>
   </si>
   <si>
@@ -424,6 +457,12 @@
   </si>
   <si>
     <t xml:space="preserve">Harjukatu 44 B 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lindroth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Johan</t>
   </si>
   <si>
     <t xml:space="preserve">010655-3210</t>
@@ -685,10 +724,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -988,10 +1027,13 @@
         <v>20</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>39800200010001</v>
+        <v>56000100010001</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>39800200010001</v>
+        <v>56000100010001</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>1</v>
@@ -1000,42 +1042,101 @@
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>19750101</v>
+        <v>19250000</v>
       </c>
       <c r="L5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>80</v>
+        <v>220</v>
       </c>
       <c r="O5" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="Q5" s="2" t="n">
-        <v>250</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="T5" s="2" t="n">
+        <v>19790101</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2" t="n">
+        <v>6738477</v>
+      </c>
+      <c r="Y5" s="2" t="n">
+        <v>452008</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>39800200010001</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>39800200010001</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>19750101</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2" t="n">
+        <v>250</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" s="2" t="n">
         <v>19780101</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="X5" s="2" t="n">
+      <c r="V6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="2" t="n">
         <v>6765134</v>
       </c>
-      <c r="Y5" s="2" t="n">
+      <c r="Y6" s="2" t="n">
         <v>428759</v>
       </c>
     </row>
@@ -1055,10 +1156,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1076,25 +1177,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1108,10 +1209,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -1120,10 +1221,10 @@
         <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
@@ -1147,10 +1248,10 @@
         <v>35</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>44</v>
@@ -1173,14 +1274,14 @@
         <v>15100</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1190,19 +1291,45 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>54</v>
+      <c r="H6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1221,10 +1348,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1242,70 +1369,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,7 +1443,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D2" s="9"/>
       <c r="F2" s="9" t="n">
@@ -1326,37 +1453,37 @@
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,7 +1494,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D3" s="9"/>
       <c r="F3" s="9" t="n">
@@ -1377,25 +1504,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
@@ -1411,7 +1538,7 @@
         <v>398</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>20100101</v>
@@ -1423,16 +1550,16 @@
         <v>30</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,28 +1567,69 @@
         <v>40</v>
       </c>
       <c r="B5" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>19980601</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>16200</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>19860101</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="2" t="n">
+      <c r="C6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>20010601</v>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J5" s="2" t="n">
+      <c r="G6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J6" s="2" t="n">
         <v>398</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>90</v>
+      <c r="K6" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1480,10 +1648,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1502,43 +1670,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1549,34 +1717,34 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="K2" s="8" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -1596,34 +1764,34 @@
         <v>398</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M3" s="9" t="n">
         <v>20200101</v>
@@ -1643,34 +1811,34 @@
         <v>398</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M4" s="9" t="n">
         <v>20210101</v>
@@ -1690,34 +1858,34 @@
         <v>398</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M5" s="9" t="n">
         <v>20220101</v>
@@ -1737,34 +1905,34 @@
         <v>398</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M6" s="9" t="n">
         <v>20220601</v>
@@ -1784,42 +1952,89 @@
         <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="K7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>19860101</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="2" t="n">
+      <c r="L8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="2" t="n">
         <v>20150401</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="N8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="O8" s="2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add test case for owner change
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="154">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -170,6 +170,12 @@
     <t xml:space="preserve">398</t>
   </si>
   <si>
+    <t xml:space="preserve">200000001A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39800200020001</t>
+  </si>
+  <si>
     <t xml:space="preserve">Osoite-numero</t>
   </si>
   <si>
@@ -355,6 +361,12 @@
   </si>
   <si>
     <t xml:space="preserve">Granström Otto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220752-848C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pohjonen Aarno Armas</t>
   </si>
   <si>
     <t xml:space="preserve">Huo-neisto-kirjain</t>
@@ -724,10 +736,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1137,6 +1149,68 @@
         <v>6765134</v>
       </c>
       <c r="Y6" s="2" t="n">
+        <v>428759</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>19750101</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2" t="n">
+        <v>250</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" s="2" t="n">
+        <v>19780101</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2" t="n">
+        <v>6765234</v>
+      </c>
+      <c r="Y7" s="2" t="n">
         <v>428759</v>
       </c>
     </row>
@@ -1156,10 +1230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1177,25 +1251,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,10 +1283,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -1221,10 +1295,10 @@
         <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
@@ -1248,10 +1322,10 @@
         <v>35</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>44</v>
@@ -1274,10 +1348,10 @@
         <v>15100</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,19 +1365,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1317,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>9</v>
@@ -1326,10 +1400,36 @@
         <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1348,10 +1448,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1369,70 +1469,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,7 +1543,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" s="9"/>
       <c r="F2" s="9" t="n">
@@ -1453,37 +1553,37 @@
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
       <c r="Q2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="S2" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1494,7 +1594,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D3" s="9"/>
       <c r="F3" s="9" t="n">
@@ -1504,25 +1604,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
@@ -1538,7 +1638,7 @@
         <v>398</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>20100101</v>
@@ -1550,16 +1650,16 @@
         <v>30</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,7 +1670,7 @@
         <v>560</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>19980601</v>
@@ -1579,25 +1679,25 @@
         <v>1</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>16200</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>19860101</v>
@@ -1611,7 +1711,7 @@
         <v>398</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>20010601</v>
@@ -1620,16 +1720,45 @@
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>20010601</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>398</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1650,8 +1779,8 @@
   </sheetPr>
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1670,43 +1799,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,34 +1846,34 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K2" s="8" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -1767,31 +1896,31 @@
         <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="F3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M3" s="9" t="n">
         <v>20200101</v>
@@ -1814,31 +1943,31 @@
         <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M4" s="9" t="n">
         <v>20210101</v>
@@ -1858,34 +1987,34 @@
         <v>398</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M5" s="9" t="n">
         <v>20220101</v>
@@ -1905,34 +2034,34 @@
         <v>398</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M6" s="9" t="n">
         <v>20220601</v>
@@ -1952,34 +2081,34 @@
         <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>19860101</v>
@@ -1999,34 +2128,34 @@
         <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>20150401</v>

</xml_diff>

<commit_message>
Fix the case in which an old habitant becomes the oldest
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="161">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -176,6 +176,12 @@
     <t xml:space="preserve">39800200020001</t>
   </si>
   <si>
+    <t xml:space="preserve">200000002A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39800200030001</t>
+  </si>
+  <si>
     <t xml:space="preserve">Osoite-numero</t>
   </si>
   <si>
@@ -369,6 +375,12 @@
     <t xml:space="preserve">Pohjonen Aarno Armas</t>
   </si>
   <si>
+    <t xml:space="preserve">130644-0434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riipinen Alexi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huo-neisto-kirjain</t>
   </si>
   <si>
@@ -487,6 +499,15 @@
   </si>
   <si>
     <t xml:space="preserve">Halmekatu 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riipinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halmekatu 13</t>
   </si>
 </sst>
 </file>
@@ -736,7 +757,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
@@ -1214,6 +1235,68 @@
         <v>428759</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>19750101</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2" t="n">
+        <v>250</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>19780101</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X8" s="2" t="n">
+        <v>6765334</v>
+      </c>
+      <c r="Y8" s="2" t="n">
+        <v>428759</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1230,10 +1313,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1251,25 +1334,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,10 +1366,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -1295,10 +1378,10 @@
         <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
@@ -1322,10 +1405,10 @@
         <v>35</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1339,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>44</v>
@@ -1348,10 +1431,10 @@
         <v>15100</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,19 +1448,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,7 +1474,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>9</v>
@@ -1400,10 +1483,10 @@
         <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>11</v>
@@ -1426,10 +1509,36 @@
         <v>35</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1448,10 +1557,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1469,70 +1578,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,7 +1652,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="9"/>
       <c r="F2" s="9" t="n">
@@ -1553,37 +1662,37 @@
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
       <c r="Q2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="S2" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,7 +1703,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D3" s="9"/>
       <c r="F3" s="9" t="n">
@@ -1604,25 +1713,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>35</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
@@ -1638,7 +1747,7 @@
         <v>398</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>20100101</v>
@@ -1650,16 +1759,16 @@
         <v>30</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,7 +1779,7 @@
         <v>560</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>19980601</v>
@@ -1679,25 +1788,25 @@
         <v>1</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>16200</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>19860101</v>
@@ -1711,7 +1820,7 @@
         <v>398</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>20010601</v>
@@ -1720,16 +1829,16 @@
         <v>1</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,8 +1848,8 @@
       <c r="B7" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>112</v>
+      <c r="C7" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>20010601</v>
@@ -1749,16 +1858,45 @@
         <v>1</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>20010601</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>398</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1777,10 +1915,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1799,43 +1937,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,34 +1984,34 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K2" s="8" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -1896,31 +2034,31 @@
         <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="F3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M3" s="9" t="n">
         <v>20200101</v>
@@ -1943,31 +2081,31 @@
         <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M4" s="9" t="n">
         <v>20210101</v>
@@ -1987,34 +2125,34 @@
         <v>398</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M5" s="9" t="n">
         <v>20220101</v>
@@ -2034,34 +2172,34 @@
         <v>398</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M6" s="9" t="n">
         <v>20220601</v>
@@ -2081,34 +2219,34 @@
         <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>19860101</v>
@@ -2128,34 +2266,34 @@
         <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>20150401</v>
@@ -2164,6 +2302,47 @@
         <v>2</v>
       </c>
       <c r="O8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>20010603</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some setup in tests. Fixed log error in a file
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -102,6 +102,10 @@
   </si>
   <si>
     <t xml:space="preserve">Koordi-naatti-varmuus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rakennus-
+Luokka</t>
   </si>
   <si>
     <t xml:space="preserve">000000000A</t>
@@ -607,7 +611,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -638,6 +642,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -753,22 +761,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA5" activeCellId="0" sqref="AA5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="22.81"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -850,13 +858,16 @@
       <c r="Z1" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="8" t="s">
         <v>27</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>20</v>
@@ -865,7 +876,7 @@
         <v>28341100010174</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>28341100010174</v>
@@ -876,8 +887,8 @@
       <c r="H2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>29</v>
+      <c r="J2" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>19700101</v>
@@ -888,14 +899,14 @@
       <c r="N2" s="2" t="n">
         <v>280</v>
       </c>
-      <c r="S2" s="8" t="s">
-        <v>30</v>
+      <c r="S2" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="T2" s="2" t="n">
         <v>19910101</v>
       </c>
-      <c r="U2" s="8" t="s">
-        <v>31</v>
+      <c r="U2" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="V2" s="2" t="n">
         <v>1</v>
@@ -912,31 +923,31 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>35</v>
+      <c r="J3" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="K3" s="2" t="n">
         <v>20000101</v>
@@ -959,14 +970,14 @@
       <c r="Q3" s="2" t="n">
         <v>600</v>
       </c>
-      <c r="S3" s="8" t="s">
-        <v>36</v>
+      <c r="S3" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="T3" s="2" t="n">
         <v>20010101</v>
       </c>
-      <c r="U3" s="8" t="s">
-        <v>37</v>
+      <c r="U3" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="V3" s="2" t="n">
         <v>1</v>
@@ -982,79 +993,79 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>38</v>
+      <c r="A4" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="D4" s="8" t="n">
+      <c r="D4" s="9" t="n">
         <v>39800100010001</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="9" t="n">
         <v>39800100010001</v>
       </c>
-      <c r="G4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="9" t="n">
+      <c r="G4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="K4" s="9" t="n">
+      <c r="K4" s="10" t="n">
         <v>19800101</v>
       </c>
-      <c r="L4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="9" t="n">
+      <c r="L4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="10" t="n">
         <v>1000</v>
       </c>
-      <c r="O4" s="9" t="n">
+      <c r="O4" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="P4" s="9" t="n">
+      <c r="P4" s="10" t="n">
         <v>1500</v>
       </c>
-      <c r="Q4" s="9" t="n">
+      <c r="Q4" s="10" t="n">
         <v>4500</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4" s="9" t="n">
+        <v>37</v>
+      </c>
+      <c r="T4" s="10" t="n">
         <v>19800101</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="X4" s="9" t="n">
+        <v>40</v>
+      </c>
+      <c r="V4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="10" t="n">
         <v>6761402</v>
       </c>
-      <c r="Y4" s="9" t="n">
+      <c r="Y4" s="10" t="n">
         <v>427353</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>20</v>
@@ -1063,7 +1074,7 @@
         <v>56000100010001</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>56000100010001</v>
@@ -1075,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>19250000</v>
@@ -1090,13 +1101,13 @@
         <v>1</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T5" s="2" t="n">
         <v>19790101</v>
       </c>
-      <c r="U5" s="8" t="s">
-        <v>44</v>
+      <c r="U5" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="V5" s="2" t="n">
         <v>1</v>
@@ -1108,15 +1119,15 @@
         <v>452008</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>20</v>
@@ -1134,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K6" s="2" t="n">
         <v>19750101</v>
@@ -1152,13 +1163,13 @@
         <v>250</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T6" s="2" t="n">
         <v>19780101</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V6" s="2" t="n">
         <v>1</v>
@@ -1175,19 +1186,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>1</v>
@@ -1196,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>19750101</v>
@@ -1214,13 +1225,13 @@
         <v>250</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T7" s="2" t="n">
         <v>19780101</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V7" s="2" t="n">
         <v>1</v>
@@ -1236,34 +1247,34 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>50</v>
+      <c r="A8" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="C8" s="8" t="n">
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="n">
         <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K8" s="2" t="n">
         <v>19750101</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="8" t="n">
         <v>1</v>
       </c>
       <c r="N8" s="2" t="n">
@@ -1276,13 +1287,13 @@
         <v>250</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T8" s="2" t="n">
         <v>19780101</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V8" s="2" t="n">
         <v>1</v>
@@ -1309,7 +1320,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1319,11 +1330,11 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1334,211 +1345,211 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="10" t="s">
         <v>55</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>29</v>
+      <c r="G2" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>27</v>
+      <c r="A3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>35</v>
+      <c r="G3" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>38</v>
+      <c r="A4" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="9" t="n">
+      <c r="C4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="10" t="n">
         <v>44</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="10" t="s">
         <v>64</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>46</v>
+      <c r="A6" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1553,7 +1564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1563,11 +1574,11 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,209 +1588,209 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="D1" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="E1" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="12" t="s">
         <v>76</v>
       </c>
+      <c r="I1" s="13" t="s">
+        <v>77</v>
+      </c>
       <c r="J1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" s="13" t="s">
         <v>78</v>
       </c>
+      <c r="K1" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="L1" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="S1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="S1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="T1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="U1" s="15" t="s">
         <v>89</v>
       </c>
+      <c r="V1" s="15" t="s">
+        <v>90</v>
+      </c>
       <c r="W1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="X1" s="14" t="s">
         <v>91</v>
       </c>
+      <c r="X1" s="15" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>26</v>
+      <c r="A2" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="F2" s="9" t="n">
+        <v>93</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="F2" s="10" t="n">
         <v>19950101</v>
       </c>
-      <c r="G2" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="G2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>94</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="8" t="s">
         <v>97</v>
       </c>
+      <c r="N2" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="O2" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>99</v>
+      <c r="Q2" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>32</v>
+      <c r="A3" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="F3" s="9" t="n">
+        <v>102</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="F3" s="10" t="n">
         <v>20220101</v>
       </c>
-      <c r="G3" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>102</v>
+      <c r="G3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>103</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>35</v>
+        <v>105</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
       </c>
-      <c r="Q3" s="9"/>
-      <c r="S3" s="9"/>
+      <c r="Q3" s="10"/>
+      <c r="S3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>38</v>
+      <c r="A4" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="9" t="n">
+      <c r="D4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="10" t="n">
         <v>20100101</v>
       </c>
-      <c r="G4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q4" s="9" t="s">
+      <c r="G4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>107</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>108</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="S4" s="9" t="s">
-        <v>108</v>
+      <c r="S4" s="10" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>40</v>
+      <c r="A5" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>560</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>19980601</v>
@@ -1787,40 +1798,40 @@
       <c r="G5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>93</v>
+      <c r="H5" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>16200</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>19860101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>46</v>
+      <c r="A6" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>398</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>20010601</v>
@@ -1828,28 +1839,28 @@
       <c r="G6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>93</v>
+      <c r="H6" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>48</v>
+      <c r="A7" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>398</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>20010601</v>
@@ -1857,46 +1868,46 @@
       <c r="G7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>93</v>
+      <c r="H7" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>50</v>
+      <c r="A8" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>116</v>
+      <c r="C8" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>20010601</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>93</v>
+      <c r="G8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="J8" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="J8" s="8" t="n">
         <v>398</v>
       </c>
-      <c r="K8" s="0" t="s">
-        <v>103</v>
+      <c r="K8" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1911,22 +1922,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="23.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,81 +1948,81 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="17" t="s">
         <v>123</v>
       </c>
+      <c r="I1" s="17" t="s">
+        <v>124</v>
+      </c>
       <c r="J1" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="N1" s="18" t="s">
         <v>126</v>
       </c>
+      <c r="O1" s="18" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>27</v>
+      <c r="A2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="G2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>130</v>
       </c>
+      <c r="I2" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="J2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="8" t="n">
+        <v>105</v>
+      </c>
+      <c r="K2" s="9" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -2024,229 +2035,229 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>38</v>
+      <c r="A3" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>45</v>
+      <c r="C3" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="H3" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>135</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>136</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="L3" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="9" t="n">
+      <c r="L3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="10" t="n">
         <v>20200101</v>
       </c>
-      <c r="N3" s="9" t="n">
+      <c r="N3" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="O3" s="9" t="n">
+      <c r="O3" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>38</v>
+      <c r="A4" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>45</v>
+      <c r="C4" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>140</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M4" s="9" t="n">
+      <c r="L4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="10" t="n">
         <v>20210101</v>
       </c>
-      <c r="N4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" s="9" t="n">
+      <c r="N4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>38</v>
+      <c r="A5" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>141</v>
+      <c r="C5" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="H5" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>146</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>147</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M5" s="9" t="n">
+      <c r="L5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="10" t="n">
         <v>20220101</v>
       </c>
-      <c r="N5" s="9" t="n">
+      <c r="N5" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="O5" s="9" t="n">
+      <c r="O5" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>38</v>
+      <c r="A6" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>141</v>
+      <c r="C6" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="H6" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="I6" s="10" t="s">
         <v>151</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>152</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" s="9" t="n">
+      <c r="L6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="10" t="n">
         <v>20220601</v>
       </c>
-      <c r="N6" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="O6" s="9" t="n">
+      <c r="N6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>40</v>
+      <c r="A7" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>19860101</v>
@@ -2259,41 +2270,41 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>46</v>
+      <c r="A8" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>20150401</v>
@@ -2306,43 +2317,43 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>50</v>
+      <c r="A9" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>158</v>
+        <v>129</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>159</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="M9" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9" s="8" t="n">
         <v>20010603</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="O9" s="8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a single test row
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="168">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -186,6 +186,18 @@
     <t xml:space="preserve">39800200030001</t>
   </si>
   <si>
+    <t xml:space="preserve">200000002C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39800200030005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111</t>
+  </si>
+  <si>
     <t xml:space="preserve">Osoite-numero</t>
   </si>
   <si>
@@ -231,7 +243,7 @@
     <t xml:space="preserve">Kirkkoäyrääntie</t>
   </si>
   <si>
-    <t xml:space="preserve">1d</t>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">ARTJÄRVI</t>
@@ -383,6 +395,12 @@
   </si>
   <si>
     <t xml:space="preserve">Riipinen Alexi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130644-0435</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyhjälä Antero Oy</t>
   </si>
   <si>
     <t xml:space="preserve">Huo-neisto-kirjain</t>
@@ -765,13 +783,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA5" activeCellId="0" sqref="AA5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y10" activeCellId="1" sqref="A9:I9 Y10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.95"/>
@@ -1306,6 +1324,68 @@
       </c>
       <c r="Y8" s="2" t="n">
         <v>428759</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>19750101</v>
+      </c>
+      <c r="L9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>250</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>19780101</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2" t="n">
+        <v>6765344</v>
+      </c>
+      <c r="Y9" s="2" t="n">
+        <v>428799</v>
       </c>
     </row>
   </sheetData>
@@ -1324,13 +1404,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.08"/>
@@ -1345,25 +1425,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,10 +1457,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -1389,10 +1469,10 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,7 +1486,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
@@ -1416,10 +1496,10 @@
         <v>36</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>44</v>
@@ -1442,10 +1522,10 @@
         <v>15100</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,19 +1539,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>9</v>
@@ -1494,10 +1574,10 @@
         <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>11</v>
@@ -1520,10 +1600,10 @@
         <v>36</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,7 +1617,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F8" s="8" t="n">
         <v>13</v>
@@ -1546,11 +1626,40 @@
         <v>36</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1568,13 +1677,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="1" sqref="A9:I9 I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
@@ -1589,70 +1698,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,7 +1772,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D2" s="10"/>
       <c r="F2" s="10" t="n">
@@ -1673,37 +1782,37 @@
         <v>1</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,7 +1823,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D3" s="10"/>
       <c r="F3" s="10" t="n">
@@ -1724,25 +1833,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>36</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
@@ -1758,7 +1867,7 @@
         <v>398</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>20100101</v>
@@ -1770,16 +1879,16 @@
         <v>31</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1899,7 @@
         <v>560</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>19980601</v>
@@ -1799,25 +1908,25 @@
         <v>1</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>16200</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>19860101</v>
@@ -1831,7 +1940,7 @@
         <v>398</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>20010601</v>
@@ -1840,16 +1949,16 @@
         <v>1</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,7 +1969,7 @@
         <v>398</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>20010601</v>
@@ -1869,16 +1978,16 @@
         <v>1</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,7 +1998,7 @@
         <v>398</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>20010601</v>
@@ -1898,16 +2007,46 @@
         <v>1</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="J8" s="8" t="n">
         <v>398</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>20010601</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>398</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1928,11 +2067,11 @@
   </sheetPr>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P9" activeCellId="1" sqref="A9:I9 P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.22"/>
@@ -1948,43 +2087,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,34 +2134,34 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K2" s="9" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -2045,31 +2184,31 @@
         <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M3" s="10" t="n">
         <v>20200101</v>
@@ -2092,31 +2231,31 @@
         <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M4" s="10" t="n">
         <v>20210101</v>
@@ -2136,34 +2275,34 @@
         <v>398</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F5" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M5" s="10" t="n">
         <v>20220101</v>
@@ -2183,34 +2322,34 @@
         <v>398</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F6" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M6" s="10" t="n">
         <v>20220601</v>
@@ -2230,34 +2369,34 @@
         <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>19860101</v>
@@ -2277,34 +2416,34 @@
         <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>20150401</v>
@@ -2324,28 +2463,28 @@
         <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F9" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M9" s="8" t="n">
         <v>20010603</v>

</xml_diff>

<commit_message>
Updated some test material - Fixed some but not all tests due to code still missing marking of kohde as expired when building is expired - Repositioned a couple of tests as they tested for things that would not be true at their original placement with current code - Added a few test error messages for easier debug - Added more test data and adjusted test numbers to match. Could not get the system to register additional residents correctly, which should be relooked at some point
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/DVV_original.xlsx
+++ b/tests/data/test_data_import/DVV_original.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R1 rakennus" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="178">
   <si>
     <t xml:space="preserve">Rakennustunnus</t>
   </si>
@@ -186,6 +186,18 @@
     <t xml:space="preserve">39800200030001</t>
   </si>
   <si>
+    <t xml:space="preserve">200000002C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39800200030002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200000002D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39800200030003</t>
+  </si>
+  <si>
     <t xml:space="preserve">Osoite-numero</t>
   </si>
   <si>
@@ -385,6 +397,18 @@
     <t xml:space="preserve">Riipinen Alexi</t>
   </si>
   <si>
+    <t xml:space="preserve">151046-9873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lauko Puolikuoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">151046-9874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kauko Täysikuoma</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huo-neisto-kirjain</t>
   </si>
   <si>
@@ -512,6 +536,30 @@
   </si>
   <si>
     <t xml:space="preserve">Halmekatu 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130644-0437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halmekatu 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130694-0534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mahtu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahtinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halmekatu 15</t>
   </si>
 </sst>
 </file>
@@ -522,7 +570,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -549,6 +597,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -611,7 +664,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -686,6 +739,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -765,13 +822,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA5" activeCellId="0" sqref="AA5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="22.95"/>
@@ -1305,6 +1362,130 @@
         <v>6765334</v>
       </c>
       <c r="Y8" s="2" t="n">
+        <v>428759</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>19750111</v>
+      </c>
+      <c r="L9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>250</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>19780101</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2" t="n">
+        <v>6765334</v>
+      </c>
+      <c r="Y9" s="2" t="n">
+        <v>428759</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>19750111</v>
+      </c>
+      <c r="L10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2" t="n">
+        <v>250</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T10" s="2" t="n">
+        <v>19780101</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X10" s="2" t="n">
+        <v>6765334</v>
+      </c>
+      <c r="Y10" s="2" t="n">
         <v>428759</v>
       </c>
     </row>
@@ -1324,13 +1505,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="23.08"/>
@@ -1345,25 +1526,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,10 +1558,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
@@ -1389,10 +1570,10 @@
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="n">
@@ -1416,10 +1597,10 @@
         <v>36</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>44</v>
@@ -1442,10 +1623,10 @@
         <v>15100</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,19 +1640,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>9</v>
@@ -1494,10 +1675,10 @@
         <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>11</v>
@@ -1520,10 +1701,10 @@
         <v>36</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F8" s="8" t="n">
         <v>13</v>
@@ -1546,10 +1727,62 @@
         <v>36</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1568,13 +1801,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="22.95"/>
@@ -1589,70 +1822,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,7 +1896,7 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D2" s="10"/>
       <c r="F2" s="10" t="n">
@@ -1673,37 +1906,37 @@
         <v>1</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>444</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>20100101</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,7 +1947,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D3" s="10"/>
       <c r="F3" s="10" t="n">
@@ -1724,25 +1957,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>36</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>20220101</v>
@@ -1758,7 +1991,7 @@
         <v>398</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>20100101</v>
@@ -1770,16 +2003,16 @@
         <v>31</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +2023,7 @@
         <v>560</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>19980601</v>
@@ -1799,25 +2032,25 @@
         <v>1</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>42</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>16200</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="P5" s="2" t="n">
         <v>19860101</v>
@@ -1831,7 +2064,7 @@
         <v>398</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>20010601</v>
@@ -1840,16 +2073,16 @@
         <v>1</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,7 +2093,7 @@
         <v>398</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>20010601</v>
@@ -1869,16 +2102,16 @@
         <v>1</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>398</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,7 +2122,7 @@
         <v>398</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>20010601</v>
@@ -1898,16 +2131,98 @@
         <v>1</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="J8" s="8" t="n">
         <v>398</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>20250101</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <v>16200</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>19860101</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>560</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>20250101</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <v>16200</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>19860101</v>
       </c>
     </row>
   </sheetData>
@@ -1926,13 +2241,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="23.22"/>
@@ -1948,43 +2263,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,34 +2310,34 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K2" s="9" t="n">
         <v>15230</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>20220101</v>
@@ -2045,31 +2360,31 @@
         <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M3" s="10" t="n">
         <v>20200101</v>
@@ -2092,31 +2407,31 @@
         <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M4" s="10" t="n">
         <v>20210101</v>
@@ -2136,34 +2451,34 @@
         <v>398</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F5" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="K5" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M5" s="10" t="n">
         <v>20220101</v>
@@ -2183,34 +2498,34 @@
         <v>398</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F6" s="10" t="n">
         <v>1</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="K6" s="1" t="n">
         <v>15100</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M6" s="10" t="n">
         <v>20220601</v>
@@ -2230,34 +2545,34 @@
         <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>19860101</v>
@@ -2277,34 +2592,34 @@
         <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M8" s="2" t="n">
         <v>20150401</v>
@@ -2324,28 +2639,28 @@
         <v>48</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F9" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M9" s="8" t="n">
         <v>20010603</v>
@@ -2354,6 +2669,88 @@
         <v>2</v>
       </c>
       <c r="O9" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="8" t="n">
+        <v>20010603</v>
+      </c>
+      <c r="N10" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O10" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>20010603</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>